<commit_message>
Adding test case count - 21
</commit_message>
<xml_diff>
--- a/MakeMyTrip/ExcelData/MakeMyTripWrite.xlsx
+++ b/MakeMyTrip/ExcelData/MakeMyTripWrite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="5580" windowWidth="13728" xWindow="0" yWindow="2472"/>
+    <workbookView activeTab="1" windowHeight="5508" windowWidth="14568" xWindow="0" yWindow="2472"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -21,34 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="21">
-  <si>
-    <t>CAB NAME</t>
-  </si>
-  <si>
-    <t>PRICE</t>
-  </si>
-  <si>
-    <t>Xylo, Ertiga</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,894</t>
-  </si>
-  <si>
-    <t>Maruti Suzuki Ertiga</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,298</t>
-  </si>
-  <si>
-    <t>Innova Crysta</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 15,155</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 20,081</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>adults-1</t>
   </si>
@@ -412,62 +385,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -477,55 +450,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>